<commit_message>
Alternative output with OFFICEDOWN
</commit_message>
<xml_diff>
--- a/inputs/data/SPECIES_CODES_AGGREGATES.xlsx
+++ b/inputs/data/SPECIES_CODES_AGGREGATES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\Working_Parties\iotc-es-generic\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFC850F-DA1B-467C-B499-8BE36DC357CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC03D944-45B7-40B2-8658-072E7CCE39E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20496E6B-4E41-4C9C-BE84-56D775C74A02}"/>
+    <workbookView xWindow="4290" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{20496E6B-4E41-4C9C-BE84-56D775C74A02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
   <si>
     <t>SPECIES_CODE</t>
   </si>
@@ -62,9 +62,6 @@
     <t>SPL</t>
   </si>
   <si>
-    <t>AG21</t>
-  </si>
-  <si>
     <t>SPN</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>MSK</t>
-  </si>
-  <si>
-    <t>SKM</t>
   </si>
   <si>
     <t>FAL</t>
@@ -444,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C239EC20-25CD-4910-8D2B-7F8EB706C30C}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,76 +519,76 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -602,31 +596,31 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
         <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -634,66 +628,18 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
         <v>15</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of NEI catches and shark drawings
</commit_message>
<xml_diff>
--- a/inputs/data/SPECIES_CODES_AGGREGATES.xlsx
+++ b/inputs/data/SPECIES_CODES_AGGREGATES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\Working_Parties\iotc-es-generic\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC03D944-45B7-40B2-8658-072E7CCE39E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E55838B-8791-4E4E-BCDA-C0A94D123F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{20496E6B-4E41-4C9C-BE84-56D775C74A02}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20496E6B-4E41-4C9C-BE84-56D775C74A02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>SPECIES_CODE</t>
   </si>
@@ -80,13 +80,58 @@
     <t>BTH</t>
   </si>
   <si>
-    <t>SHM</t>
-  </si>
-  <si>
     <t>THR</t>
   </si>
   <si>
     <t>PTH</t>
+  </si>
+  <si>
+    <t>SPECIES</t>
+  </si>
+  <si>
+    <t>SPECIES_NEI</t>
+  </si>
+  <si>
+    <t>Blue shark</t>
+  </si>
+  <si>
+    <t>Oceanic whitetip shark</t>
+  </si>
+  <si>
+    <t>Scalloped hammerhead</t>
+  </si>
+  <si>
+    <t>Shortfin mako</t>
+  </si>
+  <si>
+    <t>Silky shark</t>
+  </si>
+  <si>
+    <t>Bigeye tresher</t>
+  </si>
+  <si>
+    <t>Pelagic tresher</t>
+  </si>
+  <si>
+    <t>Blue shark, shortfin mako, oceanic whitetip shark</t>
+  </si>
+  <si>
+    <t>Mako sharks</t>
+  </si>
+  <si>
+    <t>Mackerel sharks,porbeagles nei</t>
+  </si>
+  <si>
+    <t>Requiem sharks nei</t>
+  </si>
+  <si>
+    <t>Various sharks nei</t>
+  </si>
+  <si>
+    <t>Hammerhead sharks nei</t>
+  </si>
+  <si>
+    <t>Thresher sharks nei</t>
   </si>
 </sst>
 </file>
@@ -438,211 +483,318 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C239EC20-25CD-4910-8D2B-7F8EB706C30C}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
+      <c r="D21" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D21">
+    <sortCondition ref="A2:A21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of BTH drawing and change in labels of years included in the report
</commit_message>
<xml_diff>
--- a/inputs/data/SPECIES_CODES_AGGREGATES.xlsx
+++ b/inputs/data/SPECIES_CODES_AGGREGATES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\Working_Parties\iotc-es-generic\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E55838B-8791-4E4E-BCDA-C0A94D123F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276654BA-A44F-4428-85EC-6EEB4E222541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20496E6B-4E41-4C9C-BE84-56D775C74A02}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20496E6B-4E41-4C9C-BE84-56D775C74A02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>